<commit_message>
Xuat chuong trinh Excel
</commit_message>
<xml_diff>
--- a/Nganh.xlsx
+++ b/Nganh.xlsx
@@ -15,21 +15,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
-  <si>
-    <t>Mã Ngành</t>
-  </si>
-  <si>
-    <t>Tên ngành</t>
-  </si>
-  <si>
-    <t>Công nghệ Thông tin</t>
-  </si>
-  <si>
-    <t>Mạng máy tính</t>
-  </si>
-  <si>
-    <t>Hệ thống thông tin quản lý</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Tên môn học</t>
+  </si>
+  <si>
+    <t>Tổng STC</t>
+  </si>
+  <si>
+    <t>Lý thuyết</t>
+  </si>
+  <si>
+    <t>Thực hành</t>
+  </si>
+  <si>
+    <t>Bắt buộc</t>
   </si>
 </sst>
 </file>
@@ -377,7 +380,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,39 +388,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="31.706543" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="13.996582" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
+    <row r="2" spans="1:6">
+      <c r="C2" t="str">
+        <f>SUM(C2:C1)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" t="str">
+        <f>SUM(D2:D1)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>SUM(E2:E1)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>